<commit_message>
added a new feature - language translation (i18n )
</commit_message>
<xml_diff>
--- a/UHI Submission Sheet- Innovation Track.xlsx
+++ b/UHI Submission Sheet- Innovation Track.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac046137/Sites/Python Projects/Innovation_challenge_4_OracleCerner_Final_submission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE12B5F-AFCA-FC40-937D-03A83E302275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895D4121-D694-B848-A151-42238E3E996F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="60">
   <si>
     <r>
       <rPr>
@@ -212,23 +212,28 @@
     <t>All the datasets we have used are provided in Github repo, further data can be added to those datasets. API's and frontend are resusable. Any change in dataset is automatically taken care in the API(backend) and hence the current data can easily be extended to include more data as and when available.</t>
   </si>
   <si>
-    <t>Only limitation today is the dataset. When new symptoms and diagnosis are added, the algorithms will automatically get extened to new use cases helping the hospital and clinic staff.</t>
-  </si>
-  <si>
     <t>Not applicable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Algorithm - Cosine Similarity.
-Improved Algorithm(if data points available) - Cosine Similarity with tf-idf weighted average </t>
-  </si>
-  <si>
-    <t>Due to limited data points, we have assumed that each symptom will equally qualify for a diagnosis but that is not the case. When we have more datapoints available (weighted average of each symptom towards a probable diagnosis), the algorithm can be further enhanced to improve the accuracy of the results provided by the algorithm. Also, we can change the method from cosine similarity to tf-idf weighted average with cosine similarities.</t>
   </si>
   <si>
     <t>Other workflows can be extended on the current principle - 
 1. Telemedicine now is where a patient can choose for an immediate session with any available provider or shedule an appointment directly to possible department.
 2. Speech to text implementation(english or local language) where symptoms are identified from text during converstion and the use the current algorithm to identify department and possible medications as well as usin
 3. Clinical decision support based on medications prescribed such as drug-drug interaction, duplicate drugs as well as environmental parameters based on patient location.</t>
+  </si>
+  <si>
+    <t>Due to limited data points, we have assumed that each symptom will equally qualify for a diagnosis but that is not the case. When we have more datapoints available (weighted average of each symptom towards a probable diagnosis), the algorithm can be further enhanced to improve the accuracy of the results provided by the algorithm. Also, we can change the method from cosine similarity to tf-idf weighted average with cosine similarities.
+We have added another experimental feature which would let the user enter the symptoms(comma seperated) in another language(current feature supports only hindi). Due to lack to time on our part, this feature doesn't have the auto suggestion which we can further added to improve the user experience.</t>
+  </si>
+  <si>
+    <t>Only limitation today is the dataset. When new symptoms and diagnosis are added, the algorithms will automatically get extened to new use cases helping the hospital and clinic staff.
+Due to less time, we have added only one language today but this can further be extended to multiple languages with speech feature as well.</t>
+  </si>
+  <si>
+    <t>1. Algorithm - Cosine Similarity.
+Improved Algorithm(if data points available) - Cosine Similarity with tf-idf weighted average 
+2. Language Support - English , Hindi
+3. Auto-suggestion symptom support - only English.
+4. Hindi language feature is experimental and needs the patient/hospital staff to enter the text in comma(,) seperated format. E.g - बुखार, चक्कर आना. This is an experimental feature and can quickly be further developed to improve patient care and experience.</t>
   </si>
 </sst>
 </file>
@@ -676,31 +681,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -709,6 +694,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -977,8 +982,8 @@
   </sheetPr>
   <dimension ref="A1:AG1042"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="201" zoomScaleNormal="201" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="201" zoomScaleNormal="201" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39:N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -986,33 +991,33 @@
     <col min="1" max="1" width="6.6640625" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="36.5" customWidth="1"/>
-    <col min="7" max="7" width="49.33203125" customWidth="1"/>
+    <col min="7" max="7" width="58" customWidth="1"/>
     <col min="8" max="8" width="26.1640625" customWidth="1"/>
     <col min="9" max="9" width="20.83203125" customWidth="1"/>
     <col min="10" max="10" width="38.83203125" customWidth="1"/>
     <col min="11" max="11" width="76.6640625" customWidth="1"/>
     <col min="12" max="12" width="38.6640625" customWidth="1"/>
     <col min="13" max="13" width="17.1640625" customWidth="1"/>
-    <col min="14" max="14" width="26.5" customWidth="1"/>
+    <col min="14" max="14" width="41" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="19" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="40"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="48"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1280,13 +1285,13 @@
       <c r="AG7" s="24"/>
     </row>
     <row r="8" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A8" s="32">
+      <c r="A8" s="43">
         <v>1</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="45" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="25" t="s">
@@ -1296,14 +1301,14 @@
         <v>20</v>
       </c>
       <c r="F8" s="26"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
-      <c r="M8" s="37"/>
-      <c r="N8" s="37"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
       <c r="O8" s="18"/>
       <c r="P8" s="18"/>
       <c r="Q8" s="18"/>
@@ -1555,13 +1560,13 @@
       <c r="AG14" s="18"/>
     </row>
     <row r="15" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A15" s="32">
+      <c r="A15" s="43">
         <v>2</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="45" t="s">
         <v>28</v>
       </c>
       <c r="D15" s="25" t="s">
@@ -1571,14 +1576,14 @@
         <v>20</v>
       </c>
       <c r="F15" s="29"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
       <c r="O15" s="18"/>
       <c r="P15" s="18"/>
       <c r="Q15" s="18"/>
@@ -1904,13 +1909,13 @@
       <c r="AG23" s="18"/>
     </row>
     <row r="24" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A24" s="32">
+      <c r="A24" s="43">
         <v>3</v>
       </c>
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="36" t="s">
+      <c r="C24" s="45" t="s">
         <v>31</v>
       </c>
       <c r="D24" s="25" t="s">
@@ -1920,14 +1925,14 @@
         <v>20</v>
       </c>
       <c r="F24" s="29"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
       <c r="O24" s="18"/>
       <c r="P24" s="18"/>
       <c r="Q24" s="18"/>
@@ -2218,13 +2223,13 @@
       <c r="AG31" s="18"/>
     </row>
     <row r="32" spans="1:33" s="31" customFormat="1" ht="13" x14ac:dyDescent="0.15">
-      <c r="A32" s="32">
+      <c r="A32" s="43">
         <v>4</v>
       </c>
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="36" t="s">
+      <c r="C32" s="45" t="s">
         <v>33</v>
       </c>
       <c r="D32" s="25" t="s">
@@ -2236,29 +2241,29 @@
       <c r="F32" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="G32" s="37" t="s">
+      <c r="G32" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="H32" s="32" t="s">
+        <v>52</v>
+      </c>
+      <c r="I32" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="J32" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="K32" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="L32" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="H32" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="I32" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="J32" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="K32" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="L32" s="37" t="s">
+      <c r="M32" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="M32" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="N32" s="37" t="s">
-        <v>57</v>
+      <c r="N32" s="32" t="s">
+        <v>59</v>
       </c>
       <c r="O32" s="18"/>
       <c r="P32" s="18"/>
@@ -2454,7 +2459,9 @@
       <c r="E37" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="F37" s="29"/>
+      <c r="F37" s="29" t="s">
+        <v>51</v>
+      </c>
       <c r="G37" s="42"/>
       <c r="H37" s="42"/>
       <c r="I37" s="42"/>
@@ -2519,30 +2526,30 @@
       <c r="AG38" s="18"/>
     </row>
     <row r="39" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A39" s="32">
+      <c r="A39" s="43">
         <v>5</v>
       </c>
-      <c r="B39" s="35" t="s">
+      <c r="B39" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="36" t="s">
+      <c r="C39" s="45" t="s">
         <v>35</v>
       </c>
       <c r="D39" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E39" s="43" t="s">
+      <c r="E39" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="F39" s="44"/>
-      <c r="G39" s="37"/>
-      <c r="H39" s="37"/>
-      <c r="I39" s="37"/>
-      <c r="J39" s="37"/>
-      <c r="K39" s="37"/>
-      <c r="L39" s="37"/>
-      <c r="M39" s="37"/>
-      <c r="N39" s="37"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="32"/>
+      <c r="K39" s="32"/>
+      <c r="L39" s="32"/>
+      <c r="M39" s="32"/>
+      <c r="N39" s="32"/>
       <c r="O39" s="18"/>
       <c r="P39" s="18"/>
       <c r="Q39" s="18"/>
@@ -2570,8 +2577,8 @@
       <c r="D40" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E40" s="45"/>
-      <c r="F40" s="46"/>
+      <c r="E40" s="37"/>
+      <c r="F40" s="38"/>
       <c r="G40" s="33"/>
       <c r="H40" s="33"/>
       <c r="I40" s="33"/>
@@ -2607,8 +2614,8 @@
       <c r="D41" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E41" s="45"/>
-      <c r="F41" s="46"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="38"/>
       <c r="G41" s="33"/>
       <c r="H41" s="33"/>
       <c r="I41" s="33"/>
@@ -2644,8 +2651,8 @@
       <c r="D42" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E42" s="47"/>
-      <c r="F42" s="48"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="40"/>
       <c r="G42" s="34"/>
       <c r="H42" s="34"/>
       <c r="I42" s="34"/>
@@ -2710,30 +2717,30 @@
       <c r="AG43" s="18"/>
     </row>
     <row r="44" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A44" s="32">
+      <c r="A44" s="43">
         <v>6</v>
       </c>
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="36" t="s">
+      <c r="C44" s="45" t="s">
         <v>38</v>
       </c>
       <c r="D44" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E44" s="43" t="s">
+      <c r="E44" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="F44" s="44"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="37"/>
-      <c r="J44" s="37"/>
-      <c r="K44" s="37"/>
-      <c r="L44" s="37"/>
-      <c r="M44" s="37"/>
-      <c r="N44" s="37"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="32"/>
+      <c r="H44" s="32"/>
+      <c r="I44" s="32"/>
+      <c r="J44" s="32"/>
+      <c r="K44" s="32"/>
+      <c r="L44" s="32"/>
+      <c r="M44" s="32"/>
+      <c r="N44" s="32"/>
       <c r="O44" s="18"/>
       <c r="P44" s="18"/>
       <c r="Q44" s="18"/>
@@ -2761,8 +2768,8 @@
       <c r="D45" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E45" s="45"/>
-      <c r="F45" s="46"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="38"/>
       <c r="G45" s="33"/>
       <c r="H45" s="33"/>
       <c r="I45" s="33"/>
@@ -2798,8 +2805,8 @@
       <c r="D46" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E46" s="45"/>
-      <c r="F46" s="46"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="38"/>
       <c r="G46" s="33"/>
       <c r="H46" s="33"/>
       <c r="I46" s="33"/>
@@ -2835,8 +2842,8 @@
       <c r="D47" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E47" s="47"/>
-      <c r="F47" s="48"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="40"/>
       <c r="G47" s="34"/>
       <c r="H47" s="34"/>
       <c r="I47" s="34"/>
@@ -2901,30 +2908,30 @@
       <c r="AG48" s="18"/>
     </row>
     <row r="49" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A49" s="32">
+      <c r="A49" s="43">
         <v>7</v>
       </c>
-      <c r="B49" s="35" t="s">
+      <c r="B49" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="C49" s="36" t="s">
+      <c r="C49" s="45" t="s">
         <v>40</v>
       </c>
       <c r="D49" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E49" s="43" t="s">
+      <c r="E49" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="F49" s="44"/>
-      <c r="G49" s="37"/>
-      <c r="H49" s="37"/>
-      <c r="I49" s="37"/>
-      <c r="J49" s="37"/>
-      <c r="K49" s="37"/>
-      <c r="L49" s="37"/>
-      <c r="M49" s="37"/>
-      <c r="N49" s="37"/>
+      <c r="F49" s="36"/>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="32"/>
+      <c r="J49" s="32"/>
+      <c r="K49" s="32"/>
+      <c r="L49" s="32"/>
+      <c r="M49" s="32"/>
+      <c r="N49" s="32"/>
       <c r="O49" s="18"/>
       <c r="P49" s="18"/>
       <c r="Q49" s="18"/>
@@ -2952,8 +2959,8 @@
       <c r="D50" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E50" s="45"/>
-      <c r="F50" s="46"/>
+      <c r="E50" s="37"/>
+      <c r="F50" s="38"/>
       <c r="G50" s="33"/>
       <c r="H50" s="33"/>
       <c r="I50" s="33"/>
@@ -2989,8 +2996,8 @@
       <c r="D51" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E51" s="45"/>
-      <c r="F51" s="46"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="38"/>
       <c r="G51" s="33"/>
       <c r="H51" s="33"/>
       <c r="I51" s="33"/>
@@ -3026,8 +3033,8 @@
       <c r="D52" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E52" s="47"/>
-      <c r="F52" s="48"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="40"/>
       <c r="G52" s="34"/>
       <c r="H52" s="34"/>
       <c r="I52" s="34"/>
@@ -3092,30 +3099,30 @@
       <c r="AG53" s="18"/>
     </row>
     <row r="54" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A54" s="32">
+      <c r="A54" s="43">
         <v>8</v>
       </c>
-      <c r="B54" s="35" t="s">
+      <c r="B54" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="C54" s="36" t="s">
+      <c r="C54" s="45" t="s">
         <v>42</v>
       </c>
       <c r="D54" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E54" s="43" t="s">
+      <c r="E54" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="F54" s="44"/>
-      <c r="G54" s="37"/>
-      <c r="H54" s="37"/>
-      <c r="I54" s="37"/>
-      <c r="J54" s="37"/>
-      <c r="K54" s="37"/>
-      <c r="L54" s="37"/>
-      <c r="M54" s="37"/>
-      <c r="N54" s="37"/>
+      <c r="F54" s="36"/>
+      <c r="G54" s="32"/>
+      <c r="H54" s="32"/>
+      <c r="I54" s="32"/>
+      <c r="J54" s="32"/>
+      <c r="K54" s="32"/>
+      <c r="L54" s="32"/>
+      <c r="M54" s="32"/>
+      <c r="N54" s="32"/>
       <c r="O54" s="18"/>
       <c r="P54" s="18"/>
       <c r="Q54" s="18"/>
@@ -3143,8 +3150,8 @@
       <c r="D55" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E55" s="45"/>
-      <c r="F55" s="46"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="38"/>
       <c r="G55" s="33"/>
       <c r="H55" s="33"/>
       <c r="I55" s="33"/>
@@ -3180,8 +3187,8 @@
       <c r="D56" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E56" s="47"/>
-      <c r="F56" s="48"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="40"/>
       <c r="G56" s="34"/>
       <c r="H56" s="34"/>
       <c r="I56" s="34"/>
@@ -3246,13 +3253,13 @@
       <c r="AG57" s="18"/>
     </row>
     <row r="58" spans="1:33" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="32">
+      <c r="A58" s="43">
         <v>9</v>
       </c>
-      <c r="B58" s="35" t="s">
+      <c r="B58" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="C58" s="36" t="s">
+      <c r="C58" s="45" t="s">
         <v>44</v>
       </c>
       <c r="D58" s="25" t="s">
@@ -3262,14 +3269,14 @@
         <v>20</v>
       </c>
       <c r="F58" s="29"/>
-      <c r="G58" s="37"/>
-      <c r="H58" s="37"/>
-      <c r="I58" s="37"/>
-      <c r="J58" s="37"/>
-      <c r="K58" s="37"/>
-      <c r="L58" s="37"/>
-      <c r="M58" s="37"/>
-      <c r="N58" s="37"/>
+      <c r="G58" s="32"/>
+      <c r="H58" s="32"/>
+      <c r="I58" s="32"/>
+      <c r="J58" s="32"/>
+      <c r="K58" s="32"/>
+      <c r="L58" s="32"/>
+      <c r="M58" s="32"/>
+      <c r="N58" s="32"/>
       <c r="O58" s="18"/>
       <c r="P58" s="18"/>
       <c r="Q58" s="18"/>
@@ -3443,13 +3450,13 @@
       <c r="AG62" s="18"/>
     </row>
     <row r="63" spans="1:33" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="32">
+      <c r="A63" s="43">
         <v>10</v>
       </c>
-      <c r="B63" s="35" t="s">
+      <c r="B63" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="C63" s="36" t="s">
+      <c r="C63" s="45" t="s">
         <v>46</v>
       </c>
       <c r="D63" s="25" t="s">
@@ -3459,14 +3466,14 @@
         <v>20</v>
       </c>
       <c r="F63" s="29"/>
-      <c r="G63" s="37"/>
-      <c r="H63" s="37"/>
-      <c r="I63" s="37"/>
-      <c r="J63" s="37"/>
-      <c r="K63" s="37"/>
-      <c r="L63" s="37"/>
-      <c r="M63" s="37"/>
-      <c r="N63" s="37"/>
+      <c r="G63" s="32"/>
+      <c r="H63" s="32"/>
+      <c r="I63" s="32"/>
+      <c r="J63" s="32"/>
+      <c r="K63" s="32"/>
+      <c r="L63" s="32"/>
+      <c r="M63" s="32"/>
+      <c r="N63" s="32"/>
       <c r="O63" s="18"/>
       <c r="P63" s="18"/>
       <c r="Q63" s="18"/>
@@ -3640,13 +3647,13 @@
       <c r="AG67" s="18"/>
     </row>
     <row r="68" spans="1:33" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="32">
+      <c r="A68" s="43">
         <v>11</v>
       </c>
-      <c r="B68" s="35" t="s">
+      <c r="B68" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C68" s="36" t="s">
+      <c r="C68" s="45" t="s">
         <v>48</v>
       </c>
       <c r="D68" s="25" t="s">
@@ -3656,14 +3663,14 @@
         <v>20</v>
       </c>
       <c r="F68" s="26"/>
-      <c r="G68" s="37"/>
-      <c r="H68" s="37"/>
-      <c r="I68" s="37"/>
-      <c r="J68" s="37"/>
-      <c r="K68" s="37"/>
-      <c r="L68" s="37"/>
-      <c r="M68" s="37"/>
-      <c r="N68" s="37"/>
+      <c r="G68" s="32"/>
+      <c r="H68" s="32"/>
+      <c r="I68" s="32"/>
+      <c r="J68" s="32"/>
+      <c r="K68" s="32"/>
+      <c r="L68" s="32"/>
+      <c r="M68" s="32"/>
+      <c r="N68" s="32"/>
       <c r="O68" s="18"/>
       <c r="P68" s="18"/>
       <c r="Q68" s="18"/>
@@ -37796,33 +37803,81 @@
     </row>
   </sheetData>
   <mergeCells count="126">
-    <mergeCell ref="M49:M52"/>
-    <mergeCell ref="N49:N52"/>
-    <mergeCell ref="E49:F52"/>
-    <mergeCell ref="G49:G52"/>
-    <mergeCell ref="H49:H52"/>
-    <mergeCell ref="I49:I52"/>
-    <mergeCell ref="J49:J52"/>
-    <mergeCell ref="K49:K52"/>
-    <mergeCell ref="L49:L52"/>
-    <mergeCell ref="M44:M47"/>
-    <mergeCell ref="N44:N47"/>
-    <mergeCell ref="E44:F47"/>
-    <mergeCell ref="G44:G47"/>
-    <mergeCell ref="H44:H47"/>
-    <mergeCell ref="I44:I47"/>
-    <mergeCell ref="J44:J47"/>
-    <mergeCell ref="K44:K47"/>
-    <mergeCell ref="L44:L47"/>
-    <mergeCell ref="M39:M42"/>
-    <mergeCell ref="N39:N42"/>
-    <mergeCell ref="E39:F42"/>
-    <mergeCell ref="G39:G42"/>
-    <mergeCell ref="H39:H42"/>
-    <mergeCell ref="I39:I42"/>
-    <mergeCell ref="J39:J42"/>
-    <mergeCell ref="K39:K42"/>
-    <mergeCell ref="L39:L42"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B22"/>
+    <mergeCell ref="C15:C22"/>
+    <mergeCell ref="A24:A30"/>
+    <mergeCell ref="B24:B30"/>
+    <mergeCell ref="C24:C30"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="C49:C52"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="A68:A73"/>
+    <mergeCell ref="B68:B73"/>
+    <mergeCell ref="C68:C73"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="L8:L13"/>
+    <mergeCell ref="M8:M13"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="G8:G13"/>
+    <mergeCell ref="H8:H13"/>
+    <mergeCell ref="I8:I13"/>
+    <mergeCell ref="N8:N13"/>
+    <mergeCell ref="J8:J13"/>
+    <mergeCell ref="K8:K13"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="L15:L21"/>
+    <mergeCell ref="M15:M21"/>
+    <mergeCell ref="N15:N21"/>
+    <mergeCell ref="G24:G30"/>
+    <mergeCell ref="H24:H30"/>
+    <mergeCell ref="I24:I30"/>
+    <mergeCell ref="J24:J30"/>
+    <mergeCell ref="K24:K30"/>
+    <mergeCell ref="L24:L30"/>
+    <mergeCell ref="M24:M30"/>
+    <mergeCell ref="N24:N30"/>
+    <mergeCell ref="G15:G21"/>
+    <mergeCell ref="H15:H21"/>
+    <mergeCell ref="I15:I21"/>
+    <mergeCell ref="J15:J21"/>
+    <mergeCell ref="K15:K21"/>
+    <mergeCell ref="K32:K37"/>
+    <mergeCell ref="L32:L37"/>
+    <mergeCell ref="M32:M37"/>
+    <mergeCell ref="N32:N37"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="C32:C37"/>
+    <mergeCell ref="G32:G37"/>
+    <mergeCell ref="H32:H37"/>
+    <mergeCell ref="I32:I37"/>
+    <mergeCell ref="J32:J37"/>
+    <mergeCell ref="M54:M56"/>
+    <mergeCell ref="N54:N56"/>
+    <mergeCell ref="E54:F56"/>
+    <mergeCell ref="G54:G56"/>
+    <mergeCell ref="H54:H56"/>
+    <mergeCell ref="I54:I56"/>
+    <mergeCell ref="J54:J56"/>
+    <mergeCell ref="K54:K56"/>
+    <mergeCell ref="L54:L56"/>
     <mergeCell ref="H58:H61"/>
     <mergeCell ref="I58:I61"/>
     <mergeCell ref="J58:J61"/>
@@ -37847,81 +37902,33 @@
     <mergeCell ref="L63:L66"/>
     <mergeCell ref="M63:M66"/>
     <mergeCell ref="N63:N66"/>
-    <mergeCell ref="M54:M56"/>
-    <mergeCell ref="N54:N56"/>
-    <mergeCell ref="E54:F56"/>
-    <mergeCell ref="G54:G56"/>
-    <mergeCell ref="H54:H56"/>
-    <mergeCell ref="I54:I56"/>
-    <mergeCell ref="J54:J56"/>
-    <mergeCell ref="K54:K56"/>
-    <mergeCell ref="L54:L56"/>
-    <mergeCell ref="K32:K37"/>
-    <mergeCell ref="L32:L37"/>
-    <mergeCell ref="M32:M37"/>
-    <mergeCell ref="N32:N37"/>
-    <mergeCell ref="A32:A37"/>
-    <mergeCell ref="B32:B37"/>
-    <mergeCell ref="C32:C37"/>
-    <mergeCell ref="G32:G37"/>
-    <mergeCell ref="H32:H37"/>
-    <mergeCell ref="I32:I37"/>
-    <mergeCell ref="J32:J37"/>
-    <mergeCell ref="L15:L21"/>
-    <mergeCell ref="M15:M21"/>
-    <mergeCell ref="N15:N21"/>
-    <mergeCell ref="G24:G30"/>
-    <mergeCell ref="H24:H30"/>
-    <mergeCell ref="I24:I30"/>
-    <mergeCell ref="J24:J30"/>
-    <mergeCell ref="K24:K30"/>
-    <mergeCell ref="L24:L30"/>
-    <mergeCell ref="M24:M30"/>
-    <mergeCell ref="N24:N30"/>
-    <mergeCell ref="G15:G21"/>
-    <mergeCell ref="H15:H21"/>
-    <mergeCell ref="I15:I21"/>
-    <mergeCell ref="J15:J21"/>
-    <mergeCell ref="K15:K21"/>
-    <mergeCell ref="L8:L13"/>
-    <mergeCell ref="M8:M13"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="C8:C13"/>
-    <mergeCell ref="G8:G13"/>
-    <mergeCell ref="H8:H13"/>
-    <mergeCell ref="I8:I13"/>
-    <mergeCell ref="N8:N13"/>
-    <mergeCell ref="J8:J13"/>
-    <mergeCell ref="K8:K13"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="A68:A73"/>
-    <mergeCell ref="B68:B73"/>
-    <mergeCell ref="C68:C73"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B15:B22"/>
-    <mergeCell ref="C15:C22"/>
-    <mergeCell ref="A24:A30"/>
-    <mergeCell ref="B24:B30"/>
-    <mergeCell ref="C24:C30"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="C49:C52"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="M39:M42"/>
+    <mergeCell ref="N39:N42"/>
+    <mergeCell ref="E39:F42"/>
+    <mergeCell ref="G39:G42"/>
+    <mergeCell ref="H39:H42"/>
+    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="J39:J42"/>
+    <mergeCell ref="K39:K42"/>
+    <mergeCell ref="L39:L42"/>
+    <mergeCell ref="M44:M47"/>
+    <mergeCell ref="N44:N47"/>
+    <mergeCell ref="E44:F47"/>
+    <mergeCell ref="G44:G47"/>
+    <mergeCell ref="H44:H47"/>
+    <mergeCell ref="I44:I47"/>
+    <mergeCell ref="J44:J47"/>
+    <mergeCell ref="K44:K47"/>
+    <mergeCell ref="L44:L47"/>
+    <mergeCell ref="M49:M52"/>
+    <mergeCell ref="N49:N52"/>
+    <mergeCell ref="E49:F52"/>
+    <mergeCell ref="G49:G52"/>
+    <mergeCell ref="H49:H52"/>
+    <mergeCell ref="I49:I52"/>
+    <mergeCell ref="J49:J52"/>
+    <mergeCell ref="K49:K52"/>
+    <mergeCell ref="L49:L52"/>
   </mergeCells>
   <conditionalFormatting sqref="E2:E1042">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">

</xml_diff>